<commit_message>
Update Schematic for review
</commit_message>
<xml_diff>
--- a/digitalSystemBoard.xlsx
+++ b/digitalSystemBoard.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19812" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +455,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -503,14 +511,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -548,9 +557,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency 2" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -854,17 +867,17 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
-    <col min="5" max="5" width="205.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="7"/>
+    <col min="5" max="5" width="205.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" customHeight="1">
@@ -897,7 +910,7 @@
       <c r="D2" s="10">
         <v>10</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1400,9 +1413,10 @@
     <hyperlink ref="C16" r:id="rId2" tooltip="https://www.digikey.com/en/supplier-centers/avx"/>
     <hyperlink ref="C12" r:id="rId3" tooltip="https://www.mouser.com/manufacturer/panasonicec/"/>
     <hyperlink ref="C28" r:id="rId4" tooltip="https://www.digikey.com/en/supplier-centers/abracon"/>
+    <hyperlink ref="E2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1414,14 +1428,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="43.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1508,7 +1522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add full footprint. Draw layout board
</commit_message>
<xml_diff>
--- a/digitalSystemBoard.xlsx
+++ b/digitalSystemBoard.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -405,14 +405,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,148 +470,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,194 +487,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -846,266 +520,24 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1113,7 +545,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1122,7 +554,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1134,60 +566,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="3">
+    <cellStyle name="Currency 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Currency 2" xfId="39"/>
-    <cellStyle name="Accent3" xfId="40" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="41" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="42" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="43" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="44" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="45" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="46" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="47" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="48" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="49" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="50" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1478,29 +866,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="55.1111111111111" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.8888888888889" style="7" customWidth="1"/>
-    <col min="3" max="3" width="46.1111111111111" style="7" customWidth="1"/>
+    <col min="1" max="1" width="55.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="7" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
-    <col min="5" max="5" width="205.222222222222" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="7"/>
+    <col min="5" max="5" width="205.28515625" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" spans="1:5">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1959,7 +1347,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" ht="18.6" customHeight="1" spans="1:5">
+    <row r="28" spans="1:5" ht="18.600000000000001" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>100</v>
       </c>
@@ -1997,7 +1385,7 @@
       <c r="A30" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="15" t="s">
         <v>109</v>
       </c>
       <c r="C30" s="13" t="s">
@@ -2014,7 +1402,7 @@
       <c r="A31" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -2063,34 +1451,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C19" r:id="rId1" display="Panasonic Electronic Components" tooltip="https://www.digikey.com/en/supplier-centers/panasonic"/>
-    <hyperlink ref="C16" r:id="rId2" display="AVX Corporation" tooltip="https://www.digikey.com/en/supplier-centers/avx"/>
-    <hyperlink ref="C12" r:id="rId3" display="Panasonic" tooltip="https://www.mouser.com/manufacturer/panasonicec/"/>
-    <hyperlink ref="C28" r:id="rId4" display="Abracon LLC" tooltip="https://www.digikey.com/en/supplier-centers/abracon"/>
+    <hyperlink ref="C19" r:id="rId1" tooltip="https://www.digikey.com/en/supplier-centers/panasonic"/>
+    <hyperlink ref="C16" r:id="rId2" tooltip="https://www.digikey.com/en/supplier-centers/avx"/>
+    <hyperlink ref="C12" r:id="rId3" tooltip="https://www.mouser.com/manufacturer/panasonicec/"/>
+    <hyperlink ref="C28" r:id="rId4" tooltip="https://www.digikey.com/en/supplier-centers/abracon"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="43.6666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.3333333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7777777777778" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3333333333333" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5555555555556" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="1" width="43.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2110,20 +1496,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" ht="18.75" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>122</v>
       </c>
@@ -2137,7 +1523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
@@ -2151,7 +1537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>126</v>
       </c>
@@ -2168,22 +1554,17 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>